<commit_message>
Tweak source xlsx for carry-right example
</commit_message>
<xml_diff>
--- a/data-ext/example-returns/Merrimack-NH-2016_carry_right.xlsx
+++ b/data-ext/example-returns/Merrimack-NH-2016_carry_right.xlsx
@@ -1247,8 +1247,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="258" zoomScaleNormal="258" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1475,7 +1475,7 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:H3"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
+  <printOptions headings="true" gridLines="true" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="0" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">

</xml_diff>